<commit_message>
- Add support for imagenet database - Performance enhancement in prepare_roidb_rpn()
</commit_message>
<xml_diff>
--- a/test-result.xlsx
+++ b/test-result.xlsx
@@ -10,13 +10,14 @@
     <sheet name="RPN" sheetId="1" r:id="rId1"/>
     <sheet name="Test" sheetId="3" r:id="rId2"/>
     <sheet name="Googlenet" sheetId="4" r:id="rId3"/>
+    <sheet name="SS" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="138">
   <si>
     <t>LOGISTIC_BBOX_TARGET</t>
   </si>
@@ -401,12 +402,6 @@
     <t>we have</t>
   </si>
   <si>
-    <t>n01735189</t>
-  </si>
-  <si>
-    <t>n03134739</t>
-  </si>
-  <si>
     <t>nxxxxx.tar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -514,6 +509,21 @@
   </si>
   <si>
     <t>labels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">FRCNN </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voc_2007_trainval.mat</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>images</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2709,7 +2719,7 @@
   <dimension ref="A1:AE54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4140,14 +4150,21 @@
     <row r="19" spans="1:30" s="3" customFormat="1"/>
     <row r="20" spans="1:30" s="3" customFormat="1"/>
     <row r="21" spans="1:30" s="3" customFormat="1"/>
-    <row r="22" spans="1:30" s="3" customFormat="1"/>
+    <row r="22" spans="1:30" s="3" customFormat="1">
+      <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" t="s">
+        <v>133</v>
+      </c>
+    </row>
     <row r="23" spans="1:30">
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24">
         <v>395909</v>
@@ -4157,7 +4174,7 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" s="7">
         <v>456567</v>
@@ -4173,41 +4190,42 @@
       <c r="A27" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="7">
-        <v>456183</v>
+      <c r="B27" s="22">
+        <v>456568</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:30">
-      <c r="I28" s="7" t="s">
-        <v>135</v>
-      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="7">
-        <v>287635</v>
+        <v>105</v>
+      </c>
+      <c r="D29" s="22">
+        <v>288661</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="7">
-        <v>393</v>
+        <v>107</v>
+      </c>
+      <c r="D30" s="22">
+        <v>107248</v>
+      </c>
+      <c r="E30" s="7">
+        <f>SUM(D29:D30)</f>
+        <v>395909</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -4216,42 +4234,26 @@
       <c r="A31" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="7">
-        <v>248</v>
+      <c r="D31" s="22">
+        <v>60658</v>
+      </c>
+      <c r="E31" s="7">
+        <f>SUM(D29:D31)</f>
+        <v>456567</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:30">
-      <c r="A32" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="22">
-        <v>107248</v>
-      </c>
-      <c r="E32" s="7">
-        <f>SUM(D29:D32)</f>
-        <v>395524</v>
-      </c>
       <c r="I32" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="22">
-        <v>60658</v>
-      </c>
-      <c r="E33" s="7">
-        <f>SUM(D29:D33)</f>
-        <v>456182</v>
-      </c>
       <c r="I33" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -4262,14 +4264,14 @@
     </row>
     <row r="35" spans="1:11">
       <c r="D35" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D36" s="7">
         <v>9928</v>
@@ -4279,7 +4281,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D37" s="7">
         <v>9948</v>
@@ -4289,7 +4291,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D38" s="7">
         <v>9939</v>
@@ -4299,7 +4301,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" s="7">
         <v>9946</v>
@@ -4309,7 +4311,7 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D40" s="7">
         <v>9990</v>
@@ -4319,16 +4321,20 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D41" s="7">
         <v>9997</v>
       </c>
+      <c r="I41" s="7">
+        <f>B25-E46</f>
+        <v>349319</v>
+      </c>
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D42" s="7">
         <v>9996</v>
@@ -4336,7 +4342,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D43" s="7">
         <v>10000</v>
@@ -4344,7 +4350,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D44" s="7">
         <v>10000</v>
@@ -4352,7 +4358,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D45" s="7">
         <v>9999</v>
@@ -4360,7 +4366,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D46" s="7">
         <v>7505</v>
@@ -4372,7 +4378,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D47" s="7">
         <v>9999</v>
@@ -4380,56 +4386,60 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D48" s="7">
         <v>10000</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D49" s="7">
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D50" s="7">
         <v>10000</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D51" s="7">
         <v>10000</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D52" s="7">
         <v>10000</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D53" s="7">
         <v>659</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="D54" s="7">
-        <f>SUM(D29,D30,D31,D36:D53)</f>
-        <v>456182</v>
+      <c r="E53" s="7">
+        <f>SUM(D47:D53)</f>
+        <v>60658</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="D54" s="7" t="e">
+        <f>SUM(D29,#REF!,#REF!,D36:D53)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -6790,4 +6800,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>